<commit_message>
reuploading testing file to workspace following amendments, ready for submission
</commit_message>
<xml_diff>
--- a/assets/read-me-files/learnpulse-manual-testing.xlsx
+++ b/assets/read-me-files/learnpulse-manual-testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RutterJ\Desktop\Full Stack Course\MS3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{931BA896-B29D-4201-93A9-74F58564031D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A15E92-0C0F-420B-9426-CAC8AD7F2626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{959469D3-F44A-46D9-9E63-330432ED82ED}"/>
   </bookViews>
@@ -208,6 +208,9 @@
     <t>Pass</t>
   </si>
   <si>
+    <t>Function taking argument in parameter passed out of search_function. This function then reads the data within the list and displays similaraly to the update_register function before exiting program.</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Noticed error with one of the lines getting cut off, string split up onto new line.
 Subsequently added new line declarations to some other print statements to add some vertical space and promote ease of reading.
@@ -236,15 +239,14 @@
 Functioning as intended, if a match is found based on trainee name, the try block is excecuted and the found row is passed out of the function as a list which can then be read by the display function.
 Except block functioning if no match is found which gives the user an option to search again or exit the program. 
 Input conversion to uppercase functional as input will accept lowercase inputs as valid.
-Data validation on choice functional as invalid commands will loop block until valid command is provided.</t>
+Data validation on choice functional as invalid commands will loop block until valid command is provided.
+Had to replace the gspread exception I wrote in with a general exception as anything more specific throws a bug, this should not affect the outcome of the code.</t>
     </r>
   </si>
   <si>
-    <t>Function taking argument in parameter passed out of search_function. This function then reads the data within the list and displays similaraly to the update_register function before exiting program.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Working as expected, called in the correct place, all other logic within working as expected to branch the program between search and input functionality.
-I added a loop after my initial testing to make the programme more user friendly in terms of the search function as generally the search functionality can be used much more quickly to glean an insight into what training data we hold for a specific person.  At the end of the search function, a while loop is initiated to ask the user for a search again or exit command. I followed the same conventions with the rest of my loops in terms of command validation and data conversion and the command from the loop is returned from the display data functionand assessed in the main function search branch inside a loop to ensure that the code properly excecutes in a loop. I have tested this with the same rigor and lowercase inputs are accepted but anything other than the specified commands are not. </t>
+    <t>Working as expected, called in the correct place, all other logic within working as expected to branch the program between search and input functionality.
+I added a loop after my initial testing to make the programme more user friendly in terms of the search function as generally the search functionality can be used much more quickly to glean an insight into what training data we hold for a specific person.  At the end of the search function, a while loop is initiated to ask the user for a search again or exit command. I followed the same conventions with the rest of my loops in terms of command validation and data conversion and the command from the loop is returned from the display data functionand assessed in the main function search branch inside a loop to ensure that the code properly excecutes in a loop. I have tested this with the same rigor and lowercase inputs are accepted but anything other than the specified commands are not. 
+Ran into a fairly significant bug before submission due to the except statement in the search function not triggering. I changed the exception to a general Exception as any other was continually throwing a bug. The loop in the search branch of this function was flawed and was not allowing clear looping of the search functionality from unsuccessful and successful search results. The code is now functional.</t>
   </si>
 </sst>
 </file>
@@ -855,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD500526-194F-440B-BB36-8A741066E6EC}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +986,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="375" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
@@ -992,7 +994,7 @@
         <v>29</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1003,10 +1005,10 @@
         <v>29</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="409.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>20</v>
       </c>

</xml_diff>